<commit_message>
Added labels for UNO terminal
</commit_message>
<xml_diff>
--- a/Eagle/Connector labels.xlsx
+++ b/Eagle/Connector labels.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petla\source\repos\Scoreboard\Eagle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94775174-B3A9-4E09-8C19-1DD99528A154}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927EC217-0998-4216-BBBD-591C6DF6CA60}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{8A9B3727-6D6B-4D2F-B2F1-C365EB0F93ED}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{8A9B3727-6D6B-4D2F-B2F1-C365EB0F93ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
     <sheet name="Scoreboard" sheetId="2" r:id="rId2"/>
+    <sheet name="Connectors UNO Terminal" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="15">
   <si>
     <t>Motherboard</t>
   </si>
@@ -69,12 +70,15 @@
   <si>
     <t>2P</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,8 +150,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +195,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,15 +354,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -345,6 +374,48 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358FDF87-2423-431A-BA6D-0BBF7AF7439F}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
@@ -1394,262 +1465,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="17">
+      <c r="A1" s="25">
         <v>1</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="17">
-        <v>2</v>
-      </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="17">
-        <v>3</v>
-      </c>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="19"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="25">
+        <v>2</v>
+      </c>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="25">
+        <v>3</v>
+      </c>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="27"/>
     </row>
     <row r="2" spans="1:23" ht="21" x14ac:dyDescent="0.5">
-      <c r="A2" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="R2" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="S2" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="T2" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="U2" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="V2" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="W2" s="23" t="s">
+      <c r="A2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="U2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="V2" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="W2" s="20" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="31" x14ac:dyDescent="0.7">
-      <c r="A5" s="17">
-        <v>4</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="17" t="s">
+      <c r="A5" s="25">
+        <v>4</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="17" t="s">
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="19"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="27"/>
     </row>
     <row r="6" spans="1:23" ht="21" x14ac:dyDescent="0.5">
-      <c r="A6" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="24"/>
-      <c r="I6" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="L6" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="M6" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="N6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="O6" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="R6" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="S6" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="T6" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="U6" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="V6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="W6" s="23" t="s">
+      <c r="A6" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="S6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="T6" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="U6" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="V6" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="W6" s="20" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="31" x14ac:dyDescent="0.7">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="17" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="27"/>
-      <c r="V9" s="27"/>
-      <c r="W9" s="27"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
     </row>
     <row r="10" spans="1:23" ht="21" x14ac:dyDescent="0.5">
-      <c r="A10" s="21">
+      <c r="A10" s="18">
         <v>1</v>
       </c>
-      <c r="B10" s="22">
-        <v>2</v>
-      </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="21">
+      <c r="B10" s="19">
+        <v>2</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="18">
         <v>1</v>
       </c>
-      <c r="J10" s="22">
-        <v>2</v>
-      </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="26"/>
-      <c r="V10" s="26"/>
-      <c r="W10" s="26"/>
+      <c r="J10" s="19">
+        <v>2</v>
+      </c>
+      <c r="K10" s="19"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1666,4 +1737,219 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B508BD70-A6C1-4938-B784-F1A94E91B27E}">
+  <dimension ref="A1:Y35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:P1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16" width="1.90625" customWidth="1"/>
+    <col min="17" max="17" width="2.7265625" customWidth="1"/>
+    <col min="18" max="21" width="3.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="30">
+        <v>12</v>
+      </c>
+      <c r="B3" s="31">
+        <v>11</v>
+      </c>
+      <c r="C3" s="32">
+        <v>10</v>
+      </c>
+      <c r="D3" s="33">
+        <v>9</v>
+      </c>
+      <c r="E3" s="33">
+        <v>8</v>
+      </c>
+      <c r="F3" s="34">
+        <v>7</v>
+      </c>
+      <c r="G3" s="30">
+        <v>6</v>
+      </c>
+      <c r="H3" s="30">
+        <v>5</v>
+      </c>
+      <c r="I3" s="30">
+        <v>4</v>
+      </c>
+      <c r="J3" s="30">
+        <v>3</v>
+      </c>
+      <c r="K3" s="30">
+        <v>2</v>
+      </c>
+      <c r="L3" s="30">
+        <v>1</v>
+      </c>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Y4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="40">
+        <v>20</v>
+      </c>
+      <c r="N5" s="40">
+        <v>19</v>
+      </c>
+      <c r="O5" s="41"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="4">
+        <v>16</v>
+      </c>
+      <c r="S5" s="8">
+        <v>15</v>
+      </c>
+      <c r="T5" s="8">
+        <v>14</v>
+      </c>
+      <c r="U5" s="28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A7" s="30">
+        <v>32</v>
+      </c>
+      <c r="B7" s="30">
+        <v>31</v>
+      </c>
+      <c r="C7" s="30">
+        <v>30</v>
+      </c>
+      <c r="D7" s="30">
+        <v>29</v>
+      </c>
+      <c r="E7" s="30">
+        <v>28</v>
+      </c>
+      <c r="F7" s="30">
+        <v>27</v>
+      </c>
+      <c r="G7" s="30">
+        <v>26</v>
+      </c>
+      <c r="H7" s="30">
+        <v>25</v>
+      </c>
+      <c r="I7" s="30">
+        <v>24</v>
+      </c>
+      <c r="J7" s="30">
+        <v>23</v>
+      </c>
+      <c r="K7" s="31">
+        <v>22</v>
+      </c>
+      <c r="L7" s="31">
+        <v>21</v>
+      </c>
+      <c r="M7" s="31">
+        <v>20</v>
+      </c>
+      <c r="N7" s="31">
+        <v>19</v>
+      </c>
+      <c r="O7" s="33">
+        <v>18</v>
+      </c>
+      <c r="P7" s="31">
+        <v>17</v>
+      </c>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" ht="12.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" ht="12.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" ht="12.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="34" ht="12.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" ht="12.9" customHeight="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>